<commit_message>
Updated Figure 3. I illustrated AC-V18 instead of AC-V09 by mistake.
</commit_message>
<xml_diff>
--- a/tables/ASCC-supplementary_table2-sample_information.xlsx
+++ b/tables/ASCC-supplementary_table2-sample_information.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26024"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-28800" yWindow="-20" windowWidth="14400" windowHeight="17540" tabRatio="500"/>
+    <workbookView xWindow="-28760" yWindow="0" windowWidth="25840" windowHeight="17540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Pilot Cohort" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="149">
   <si>
     <t>Individual ID</t>
   </si>
@@ -473,7 +473,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -497,6 +497,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -515,7 +522,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="11">
+  <cellStyleXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -527,21 +534,42 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="11">
+  <cellStyles count="21">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -873,8 +901,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="M21" sqref="M21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -892,6 +920,7 @@
     <col min="11" max="11" width="23.33203125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="23.6640625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="25" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="20.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
@@ -1636,6 +1665,12 @@
         <v>40245334</v>
       </c>
       <c r="K20" t="s">
+        <v>142</v>
+      </c>
+      <c r="L20" t="s">
+        <v>142</v>
+      </c>
+      <c r="M20" t="s">
         <v>142</v>
       </c>
     </row>
@@ -1655,7 +1690,7 @@
   <dimension ref="A1:J46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1668,6 +1703,7 @@
     <col min="6" max="6" width="18" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.1640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="32" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="32.6640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="26" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2092,29 +2128,31 @@
       </c>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" t="s">
+      <c r="A19" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B19" t="s">
-        <v>47</v>
-      </c>
-      <c r="D19" t="s">
-        <v>35</v>
-      </c>
-      <c r="E19" t="s">
-        <v>30</v>
-      </c>
-      <c r="F19" t="s">
-        <v>33</v>
-      </c>
-      <c r="G19" t="s">
+      <c r="B19" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G19" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="H19">
-        <v>63.338282999999997</v>
-      </c>
-      <c r="J19">
-        <v>36036321</v>
+      <c r="H19" s="1">
+        <v>76.882260000000002</v>
+      </c>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1">
+        <v>34962621</v>
       </c>
     </row>
     <row r="20" spans="1:10">
@@ -2122,10 +2160,10 @@
         <v>46</v>
       </c>
       <c r="B20" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D20" t="s">
-        <v>12</v>
+        <v>35</v>
       </c>
       <c r="E20" t="s">
         <v>30</v>
@@ -2137,10 +2175,10 @@
         <v>27</v>
       </c>
       <c r="H20">
-        <v>76.882260000000002</v>
+        <v>63.338282999999997</v>
       </c>
       <c r="J20">
-        <v>34962621</v>
+        <v>36036321</v>
       </c>
     </row>
     <row r="21" spans="1:10">

</xml_diff>